<commit_message>
corrected bom qty for 10pF caps (3x)
</commit_message>
<xml_diff>
--- a/bill-of-materials/photon-bom-v019.xlsx
+++ b/bill-of-materials/photon-bom-v019.xlsx
@@ -610,8 +610,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -621,6 +619,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,10 +993,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="14" t="s">
         <v>99</v>
       </c>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="14" t="s">
         <v>103</v>
       </c>
@@ -1067,7 +1067,7 @@
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="21" t="s">
         <v>104</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1172,15 +1172,15 @@
       <c r="G10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="24"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>

</xml_diff>